<commit_message>
ajuste chatbot y data
</commit_message>
<xml_diff>
--- a/data/Anomalias Robos Nestle.xlsx
+++ b/data/Anomalias Robos Nestle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilspglobalsegu-my.sharepoint.com/personal/erivas_ai27_com/Documents/Documentos/Areas de Trabajo/Inteligencia de Negocios/Aplicaciones/App Nestle/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilspglobalsegu-my.sharepoint.com/personal/erivas_ai27_com/Documents/Documentos/Areas de Trabajo/Inteligencia de Negocios/Aplicaciones/Productivo/RiesgoNestle/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6923E592-EB80-464C-9E63-7ED0061706D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C19A3469-A15C-46DF-B566-C008C08137E9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{6923E592-EB80-464C-9E63-7ED0061706D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0B5220B-7654-4613-B777-A665AE2FF9EF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2A1D726-0224-43C7-9055-C4E2B53271AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2A1D726-0224-43C7-9055-C4E2B53271AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5907" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6042" uniqueCount="1275">
   <si>
     <t>UNIDAD EN ESPERA DE MAS INFORMACION POR PARTE DE LT   /// NC   TTYL 22 - 94AC5M WIDGETS UBICACIÓN HACE 11 MINUTOS (19/09/2023 21:26) ANILLO PERIFÉRICO ORIENTE MANUEL GÓMEZ MORÍN, SAN JOSÉ EL 15, EL SALTO, JALISCO, MÉXICO, 45659 20.530325, -103.272159 (ALTITUD 1547 METROS) VELOCIDAD: 0 KM/H</t>
   </si>
@@ -6466,6 +6466,117 @@
   </si>
   <si>
     <t>Bitácora</t>
+  </si>
+  <si>
+    <t>7A5190613</t>
+  </si>
+  <si>
+    <t>M100612151</t>
+  </si>
+  <si>
+    <t>TRUCKMAN</t>
+  </si>
+  <si>
+    <t>PORFIRIO FRANCISCO ORTIGOZA MALDONADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUADALUPE NUEVO LEON </t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE MIARADORES-LAS VIGAS,  INFORMA OPERADOR QUE SE DETIENE POR FALLA MECÁNICA  (MANGUERA DE COMBUSTIBLE REVENTADA) Y BRINDA CLAVE DE AMAGO INCORRECTA, SE LE SUGIERE PARO DE MOTOR A OPERADOR Y A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA..// 6 MIN 24 S AGO  MEX-140D, TLACOLULAN, VERACRUZ DE IGNACIO DE LA LLAVE, MEXICO   12:36 51 MIN</t>
+  </si>
+  <si>
+    <t>7A5191712</t>
+  </si>
+  <si>
+    <t>REFRIGERADOS TREEEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAFAEL ORTIZ </t>
+  </si>
+  <si>
+    <t>ESTADÍA NO AUTORIZADA POR SANITARIO</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE     IXTLAHUACA CENTRO  INFORMA OPERADOR QUE SE DETIENE POR   SANITARIO  Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SUGIERE PARO DE MOTOR  A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA VÍA WHATSAPP.   39 S AGO  MEX-15D, IXTLAHUACA CENTRO, IXTLAHUACA, MÉXICO 50740, MEXICO     0 KM/H 09:12 1 H 16 MIN 38.75 KM</t>
+  </si>
+  <si>
+    <t>7A5198767</t>
+  </si>
+  <si>
+    <t>NOE SILGUERO FLORES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD SE VISUALIZA EN RUTA SOBRE   LIBRAMIENTO ACAMBAY , SE ENLAZA CON OP INDICA DESVÍO POR AUTORIZACION DE LT , Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SOLICITA ESTATUS A LT VÍA WHATSAPP EN ESPERA DE MÁS INFORMACIÓN     NAME: 2045 LOCATION: LIB. A QUERÉTARO, 50334 MÉX., MEXICO 19.940321,-99.858436 STATUS: DRIVING SINCE 10/11/23 10:46:36 AM SPEED: 58 MPH </t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE  SLP´-MATEHUALA KM 156 SANTA MARIA DEL RIO   INFORMA OPERADOR QUE SE DETIENE POR    Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SUGIERE PARO DE MOTOR  A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA VÍA WHATSAPP.    9 MIN 18 S AGO  CALLE LÁZARO CÁRDENAS DEL RÍO, LOMA BONITA, SANTA MARÍA DEL RÍO, SAN LUIS POTOSÍ 79560, MEXICO   16:11 45 MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SE VISUALIZA UNIDAD DETENIDA SOBRE  SLP-MATEHUALA KM 74   OPERADOR NO CONTESTA, SE LE SOLICITA PARO DE MOTOR Y ESTATUS A LÍNEA TRANSPORTISTA VÍA WHATSAPP.  1 MIN AGO  MEX-57, GUADALCÁZAR, SAN LUIS POTOSÍ, MEXICO   19:18 20 MIN</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE QUERETARO-SLP KM44, GTO; OPERADOR NO CONTESTA SE LE SOLICITA PARO DE MOTOR Y ESTATUS A LÍNEA TRANSPORTISTA VÍA WHATSAPP. SE SOLICITA RESET DE CE. // ↬MHO↫ NAME: 2045 LOCATION: SAN LUIS POTOSÍ - SANTIAGO DE QUERÉTARO 119, 37987 GTO., MEXICO STATUS: STOPPED SINCE 10/11/23 01:32:59 PM SPEED: 0 MPH</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE MATEHUALA-MONTERREY KM120, NL; OPERADOR NO CONTESTA SE LE SOLICITA PARO DE MOTOR Y ESTATUS A LÍNEA TRANSPORTISTA VÍA WHATSAPP. // ↬MHO↫ 39 MIN AGO  MEX-57, GALEANA, NUEVO LEÓN, MEXICO 23:24 39 MIN</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE MATEHUALA-MONTERREY KM234, COAH; OPERADOR NO CONTESTA SE LE SOLICITA PARO DE MOTOR Y ESTATUS A LÍNEA TRANSPORTISTA VÍA WHATSAPP. // ↬MHO↫ 4 MIN 8 S AGO  MEX-57D, ARTEAGA, COAHUILA DE ZARAGOZA, MEXICO  0 KM/H 03:55 1 MIN 55 S 0.00 KM</t>
+  </si>
+  <si>
+    <t>7A5201293</t>
+  </si>
+  <si>
+    <t>M100612409</t>
+  </si>
+  <si>
+    <t>PAULO HUMBERTO SIQUEIROS</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE , CARRETERA SAN JUAN DEL RÍO-ATLACOMULCO, SAN JUAN DEL RÍO ESTADO: QRO,  KM 130, A LA ALTURAD E LA CASETA DE PALMILLAS.  INFORMA OPERADOR QUE SE DETIENE POR  UN CAFE Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SUGIERE PARO DE MOTOR A OPERADOR Y A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA.🚓✅   46 S AGO  MEX-55, SAN JUAN DEL RÍO, QUERÉTARO, MEXICO   06:09 7 MIN 0 S</t>
+  </si>
+  <si>
+    <t>UNIDAD SE VISUALIZA DETENIDA SOBRE  CARRETERA LEÓN-AGUASCALIENTES COLONIA: MUNICIPIO: LEÓN, PASANDO CASETA LEON, OP NO RESPONDE MEDIO, SE PIDE ESTATUS A LT POR WA//15 S AGO  CARRETERA LEÓN-AGUASCALIENTES, LEÓN, GUANAJUATO, MEXICO   10:43 1 H 30 MIN</t>
+  </si>
+  <si>
+    <t>7A5217583</t>
+  </si>
+  <si>
+    <t>M100614267</t>
+  </si>
+  <si>
+    <t>MAX LILIAN PALMA</t>
+  </si>
+  <si>
+    <t>SORIANA NUEVO LEON</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE  QUERÉTARO ESTADO: QRO, OPERADOR NO CONTESTA, SE LE SOLICITA PARO DE MOTOR Y ESTATUS A LÍNEA TRANSPORTISTA VÍA WHATSAPP. // - ALIAS: TR097 - ÚLTIMA POSICIÓN: 2023-10-18 02:30:27  - LOCALIZACIÓN: JOFRITO,QUERÉTARO, QUERETARO - ESTATUS / DURACIÓN: OCIOSO 12M 2S - VELOCIDAD: 0.0 KM/H - COORDENADAS: 20.8403041,-100.4374415</t>
+  </si>
+  <si>
+    <t>7A5228296</t>
+  </si>
+  <si>
+    <t>JOSE LUIS ROSALES PEREZ</t>
+  </si>
+  <si>
+    <t>SE VISUALIZA UNIDAD DETENIDA SOBRE MATEHUALA - SAN LUIS POTOSI , INFORMA OPERADOR QUE SE DETIENE POR RESGUARDO YA QUE LO VENIA SIGUEN UN JETA BLANCO DESDE LA BAJADA SAN LUIS POTOSI  Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SUGIERE PARO DE MOTOR A OPERADOR Y A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA.  SAN LORENZO, 78973 S.L.P., MEXICO 22.568985,22.568985 DESTINATION: PROL. GUADALUPE GARCÍA 3918, 150 ANIVERSARIO, 88283 NUEVO LAREDO, TAMPS., MEXICO ETA: 7H 23M</t>
+  </si>
+  <si>
+    <t>7A5233215</t>
+  </si>
+  <si>
+    <t>M100617806</t>
+  </si>
+  <si>
+    <t>ERICK MARTINEZ MARIN</t>
+  </si>
+  <si>
+    <t>CEDIS WALMART CIENEGA DE FLORES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE VISUALIZA UNIDAD DETENIDA SOBRE ,  INFORMA OPERADOR VIA TC 8087 QUE SE DETIENE POR SANITARIO Y BRINDA CLAVE DE AMAGO CORRECTA, SE LE SUGIERE PARO DE MOTOR A OPERADOR Y A LÍNEA TRANSPORTISTA, SE SOLICITA EVIDENCIA, SE SOLICITA A OPERADOR Y LT VIA WA RESGUARDARSE EN UNA PENSION CERRADA O PATIOS DE LT  Y NO CIRCULAR EN ESTE HORARIO /// (¬_¬) CFCS  AT-6041 TOLUCA  2022 KENWORTH T680·  AUTORIZADA. ESTACION DE SERVICIO SANTA MARIA DEL RIO, SLP SANTA MARÍA DEL RÍO, SLP, 79560 24 DE OCT. DE 2023 03: </t>
   </si>
 </sst>
 </file>
@@ -6909,9 +7020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2036FB5C-5D49-4069-AF4C-05037FE4002D}">
-  <dimension ref="A1:P589"/>
+  <dimension ref="A1:P602"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
+      <selection activeCell="F592" sqref="F592"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36332,6 +36445,656 @@
         <v>0</v>
       </c>
     </row>
+    <row r="590" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A590" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B590" t="s">
+        <v>38</v>
+      </c>
+      <c r="C590" s="10" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D590" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E590" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F590" t="s">
+        <v>34</v>
+      </c>
+      <c r="G590" t="s">
+        <v>33</v>
+      </c>
+      <c r="H590" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I590" t="s">
+        <v>86</v>
+      </c>
+      <c r="J590" s="3">
+        <v>690</v>
+      </c>
+      <c r="K590" s="3">
+        <v>12</v>
+      </c>
+      <c r="L590" t="s">
+        <v>41</v>
+      </c>
+      <c r="M590">
+        <v>19.641590000000001</v>
+      </c>
+      <c r="N590">
+        <v>-96.983979000000005</v>
+      </c>
+      <c r="O590" s="7">
+        <v>45207.567348923614</v>
+      </c>
+      <c r="P590" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="591" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A591" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B591" t="s">
+        <v>17</v>
+      </c>
+      <c r="C591" s="10">
+        <v>4573644620</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E591" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F591" t="s">
+        <v>44</v>
+      </c>
+      <c r="G591" t="s">
+        <v>23</v>
+      </c>
+      <c r="H591" t="s">
+        <v>13</v>
+      </c>
+      <c r="I591" t="s">
+        <v>12</v>
+      </c>
+      <c r="J591" s="3">
+        <v>50</v>
+      </c>
+      <c r="K591" s="3">
+        <v>2</v>
+      </c>
+      <c r="L591" t="s">
+        <v>1247</v>
+      </c>
+      <c r="M591">
+        <v>19.57423</v>
+      </c>
+      <c r="N591">
+        <v>-99.760733000000002</v>
+      </c>
+      <c r="O591" s="7">
+        <v>45210.396989351852</v>
+      </c>
+      <c r="P591" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="592" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A592" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B592" t="s">
+        <v>17</v>
+      </c>
+      <c r="C592" s="10">
+        <v>4573626834</v>
+      </c>
+      <c r="D592" t="s">
+        <v>46</v>
+      </c>
+      <c r="E592" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F592" t="s">
+        <v>126</v>
+      </c>
+      <c r="G592" t="s">
+        <v>23</v>
+      </c>
+      <c r="H592" t="s">
+        <v>13</v>
+      </c>
+      <c r="I592" t="s">
+        <v>12</v>
+      </c>
+      <c r="J592" s="3">
+        <v>50</v>
+      </c>
+      <c r="K592" s="3">
+        <v>2</v>
+      </c>
+      <c r="L592" t="s">
+        <v>212</v>
+      </c>
+      <c r="M592">
+        <v>19.940321000000001</v>
+      </c>
+      <c r="N592">
+        <v>-99.858435999999998</v>
+      </c>
+      <c r="O592" s="7">
+        <v>45210.459944560185</v>
+      </c>
+      <c r="P592" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="593" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A593" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B593" t="s">
+        <v>17</v>
+      </c>
+      <c r="C593" s="10">
+        <v>4573644620</v>
+      </c>
+      <c r="D593" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E593" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F593" t="s">
+        <v>44</v>
+      </c>
+      <c r="G593" t="s">
+        <v>23</v>
+      </c>
+      <c r="H593" t="s">
+        <v>13</v>
+      </c>
+      <c r="I593" t="s">
+        <v>12</v>
+      </c>
+      <c r="J593" s="3">
+        <v>50</v>
+      </c>
+      <c r="K593" s="3">
+        <v>2</v>
+      </c>
+      <c r="L593" t="s">
+        <v>11</v>
+      </c>
+      <c r="M593">
+        <v>21.806863</v>
+      </c>
+      <c r="N593">
+        <v>-100.724232</v>
+      </c>
+      <c r="O593" s="7">
+        <v>45210.669389155089</v>
+      </c>
+      <c r="P593" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="594" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A594" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B594" t="s">
+        <v>17</v>
+      </c>
+      <c r="C594" s="10">
+        <v>4573644620</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E594" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F594" t="s">
+        <v>44</v>
+      </c>
+      <c r="G594" t="s">
+        <v>23</v>
+      </c>
+      <c r="H594" t="s">
+        <v>13</v>
+      </c>
+      <c r="I594" t="s">
+        <v>12</v>
+      </c>
+      <c r="J594" s="3">
+        <v>50</v>
+      </c>
+      <c r="K594" s="3">
+        <v>2</v>
+      </c>
+      <c r="L594" t="s">
+        <v>11</v>
+      </c>
+      <c r="M594">
+        <v>22.631907000000002</v>
+      </c>
+      <c r="N594">
+        <v>-100.523946</v>
+      </c>
+      <c r="O594" s="7">
+        <v>45210.780100428237</v>
+      </c>
+      <c r="P594" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="595" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A595" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B595" t="s">
+        <v>17</v>
+      </c>
+      <c r="C595" s="10">
+        <v>4573626834</v>
+      </c>
+      <c r="D595" t="s">
+        <v>46</v>
+      </c>
+      <c r="E595" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F595" t="s">
+        <v>126</v>
+      </c>
+      <c r="G595" t="s">
+        <v>23</v>
+      </c>
+      <c r="H595" t="s">
+        <v>13</v>
+      </c>
+      <c r="I595" t="s">
+        <v>12</v>
+      </c>
+      <c r="J595" s="3">
+        <v>50</v>
+      </c>
+      <c r="K595" s="3">
+        <v>2</v>
+      </c>
+      <c r="L595" t="s">
+        <v>11</v>
+      </c>
+      <c r="M595">
+        <v>20.9542</v>
+      </c>
+      <c r="N595">
+        <v>-100.42310000000001</v>
+      </c>
+      <c r="O595" s="7">
+        <v>45210.86228105324</v>
+      </c>
+      <c r="P595" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="596" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A596" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B596" t="s">
+        <v>17</v>
+      </c>
+      <c r="C596" s="10">
+        <v>4573644620</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E596" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F596" t="s">
+        <v>44</v>
+      </c>
+      <c r="G596" t="s">
+        <v>23</v>
+      </c>
+      <c r="H596" t="s">
+        <v>13</v>
+      </c>
+      <c r="I596" t="s">
+        <v>12</v>
+      </c>
+      <c r="J596" s="3">
+        <v>50</v>
+      </c>
+      <c r="K596" s="3">
+        <v>2</v>
+      </c>
+      <c r="L596" t="s">
+        <v>11</v>
+      </c>
+      <c r="M596">
+        <v>24.603515999999999</v>
+      </c>
+      <c r="N596">
+        <v>-100.27099200000001</v>
+      </c>
+      <c r="O596" s="7">
+        <v>45210.969183333335</v>
+      </c>
+      <c r="P596" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="597" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A597" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B597" t="s">
+        <v>17</v>
+      </c>
+      <c r="C597" s="10">
+        <v>4573644620</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E597" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F597" t="s">
+        <v>44</v>
+      </c>
+      <c r="G597" t="s">
+        <v>23</v>
+      </c>
+      <c r="H597" t="s">
+        <v>13</v>
+      </c>
+      <c r="I597" t="s">
+        <v>12</v>
+      </c>
+      <c r="J597" s="3">
+        <v>50</v>
+      </c>
+      <c r="K597" s="3">
+        <v>2</v>
+      </c>
+      <c r="L597" t="s">
+        <v>11</v>
+      </c>
+      <c r="M597">
+        <v>25.426162999999999</v>
+      </c>
+      <c r="N597">
+        <v>-100.80515200000001</v>
+      </c>
+      <c r="O597" s="7">
+        <v>45211.129068865739</v>
+      </c>
+      <c r="P597" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="598" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A598" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B598" t="s">
+        <v>38</v>
+      </c>
+      <c r="C598" s="10" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D598" t="s">
+        <v>36</v>
+      </c>
+      <c r="E598" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F598" t="s">
+        <v>126</v>
+      </c>
+      <c r="G598" t="s">
+        <v>23</v>
+      </c>
+      <c r="H598" t="s">
+        <v>51</v>
+      </c>
+      <c r="I598" t="s">
+        <v>2</v>
+      </c>
+      <c r="J598" s="3">
+        <v>813</v>
+      </c>
+      <c r="K598" s="3">
+        <v>14</v>
+      </c>
+      <c r="L598" t="s">
+        <v>11</v>
+      </c>
+      <c r="M598">
+        <v>20.284127000000002</v>
+      </c>
+      <c r="N598">
+        <v>-99.931297999999998</v>
+      </c>
+      <c r="O598" s="7">
+        <v>45211.268226307868</v>
+      </c>
+      <c r="P598" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="599" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A599" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B599" t="s">
+        <v>38</v>
+      </c>
+      <c r="C599" s="10" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D599" t="s">
+        <v>36</v>
+      </c>
+      <c r="E599" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F599" t="s">
+        <v>126</v>
+      </c>
+      <c r="G599" t="s">
+        <v>23</v>
+      </c>
+      <c r="H599" t="s">
+        <v>51</v>
+      </c>
+      <c r="I599" t="s">
+        <v>2</v>
+      </c>
+      <c r="J599" s="3">
+        <v>813</v>
+      </c>
+      <c r="K599" s="3">
+        <v>14</v>
+      </c>
+      <c r="L599" t="s">
+        <v>11</v>
+      </c>
+      <c r="M599">
+        <v>21.109655</v>
+      </c>
+      <c r="N599">
+        <v>-101.793758</v>
+      </c>
+      <c r="O599" s="7">
+        <v>45211.51326446759</v>
+      </c>
+      <c r="P599" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="600" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A600" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B600" t="s">
+        <v>38</v>
+      </c>
+      <c r="C600" s="10" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D600" t="s">
+        <v>942</v>
+      </c>
+      <c r="E600" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F600" t="s">
+        <v>126</v>
+      </c>
+      <c r="G600" t="s">
+        <v>23</v>
+      </c>
+      <c r="H600" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I600" t="s">
+        <v>86</v>
+      </c>
+      <c r="J600" s="3">
+        <v>597</v>
+      </c>
+      <c r="K600" s="3">
+        <v>11</v>
+      </c>
+      <c r="L600" t="s">
+        <v>11</v>
+      </c>
+      <c r="M600">
+        <v>20.840306000000002</v>
+      </c>
+      <c r="N600">
+        <v>-100.437461</v>
+      </c>
+      <c r="O600" s="7">
+        <v>45217.10862071759</v>
+      </c>
+      <c r="P600" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="601" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A601" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B601" t="s">
+        <v>17</v>
+      </c>
+      <c r="C601" s="10">
+        <v>4573738806</v>
+      </c>
+      <c r="D601" t="s">
+        <v>46</v>
+      </c>
+      <c r="E601" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F601" t="s">
+        <v>126</v>
+      </c>
+      <c r="G601" t="s">
+        <v>23</v>
+      </c>
+      <c r="H601" t="s">
+        <v>13</v>
+      </c>
+      <c r="I601" t="s">
+        <v>12</v>
+      </c>
+      <c r="J601" s="3">
+        <v>50</v>
+      </c>
+      <c r="K601" s="3">
+        <v>2</v>
+      </c>
+      <c r="L601" t="s">
+        <v>11</v>
+      </c>
+      <c r="M601">
+        <v>22.569247000000001</v>
+      </c>
+      <c r="N601">
+        <v>-100.63384499999999</v>
+      </c>
+      <c r="O601" s="7">
+        <v>45220.737899918982</v>
+      </c>
+      <c r="P601" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="602" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A602" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B602" t="s">
+        <v>38</v>
+      </c>
+      <c r="C602" s="10" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D602" t="s">
+        <v>248</v>
+      </c>
+      <c r="E602" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F602" t="s">
+        <v>126</v>
+      </c>
+      <c r="G602" t="s">
+        <v>23</v>
+      </c>
+      <c r="H602" t="s">
+        <v>1273</v>
+      </c>
+      <c r="I602" t="s">
+        <v>86</v>
+      </c>
+      <c r="J602" s="3">
+        <v>597</v>
+      </c>
+      <c r="K602" s="3">
+        <v>11</v>
+      </c>
+      <c r="L602" t="s">
+        <v>11</v>
+      </c>
+      <c r="M602">
+        <v>21.807006000000001</v>
+      </c>
+      <c r="N602">
+        <v>-100.72333999999999</v>
+      </c>
+      <c r="O602" s="7">
+        <v>45223.153292129631</v>
+      </c>
+      <c r="P602" t="s">
+        <v>1274</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>